<commit_message>
0.1.5: ant task option "client" is implementd to avoid generate service methods.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FC6D5A-C868-7242-B4D0-222979C1CFE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744CF73E-76B5-9548-B9B9-7AFF9A392783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">config!$C$5:$C$6</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -271,6 +271,23 @@
   </si>
   <si>
     <t>API定義書からAPIスタブクラスを自動生成するBlancoRestGeneratorTsのためのAntTaskです。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>client</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>trueの場合はサーバ用のメソッドを生成しません。</t>
+    <rPh sb="5" eb="7">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t xml:space="preserve">ヨウ </t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t xml:space="preserve">セイセイシマセン。 </t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1217,7 +1234,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1261,7 +1278,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1289,7 +1306,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1629,12 +1646,22 @@
       <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
+      <c r="A22" s="27">
+        <v>9</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="D22" s="29"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31"/>
+      <c r="E22" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>49</v>
+      </c>
       <c r="G22" s="31"/>
       <c r="H22" s="31"/>
       <c r="I22" s="31"/>

</xml_diff>

<commit_message>
0.1.5, 0.1.6: Enable specifing white space numbers for a tab.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744CF73E-76B5-9548-B9B9-7AFF9A392783}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7807B6-A886-D847-A6DC-039C191FB71C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -287,6 +287,33 @@
     </rPh>
     <rPh sb="18" eb="20">
       <t xml:space="preserve">セイセイシマセン。 </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>tabs</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>整数(int)</t>
+    <rPh sb="0" eb="2">
+      <t>セイスウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>タブをwhite spaceいくつで置き換えるか、という値です。</t>
+    <rPh sb="0" eb="2">
+      <t>ジドウ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>モジ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>シテイ</t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -732,7 +759,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -843,6 +870,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1234,7 +1266,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1278,7 +1310,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1303,10 +1335,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F22" sqref="F22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1511,7 +1543,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="27">
-        <f t="shared" ref="A16:A21" si="0">A15+1</f>
+        <f t="shared" ref="A16:A22" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="28" t="s">
@@ -1576,23 +1608,23 @@
       <c r="I18" s="50"/>
       <c r="J18" s="32"/>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="27">
+    <row r="19" spans="1:10" s="70" customFormat="1">
+      <c r="A19" s="68">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B19" s="51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="57" t="s">
-        <v>40</v>
+      <c r="B19" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="49">
+        <v>4</v>
+      </c>
+      <c r="F19" s="69" t="s">
+        <v>52</v>
       </c>
       <c r="G19" s="50"/>
       <c r="H19" s="50"/>
@@ -1601,79 +1633,90 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="27">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B20" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="45" t="s">
-        <v>33</v>
+        <f>A18+1</f>
+        <v>6</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>34</v>
       </c>
       <c r="D20" s="52"/>
-      <c r="E20" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="58" t="s">
-        <v>31</v>
+      <c r="E20" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="57" t="s">
+        <v>40</v>
       </c>
       <c r="G20" s="50"/>
       <c r="H20" s="50"/>
       <c r="I20" s="50"/>
       <c r="J20" s="32"/>
     </row>
-    <row r="21" spans="1:10" ht="63" customHeight="1">
+    <row r="21" spans="1:10">
       <c r="A21" s="27">
         <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B21" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="52"/>
+      <c r="E21" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="32"/>
+    </row>
+    <row r="22" spans="1:10" ht="63" customHeight="1">
+      <c r="A22" s="27">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B21" s="51" t="s">
+      <c r="B22" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C22" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="56" t="s">
+      <c r="D22" s="52"/>
+      <c r="E22" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="F21" s="59" t="s">
+      <c r="F22" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="32"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="27">
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="32"/>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="27">
         <v>9</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B23" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C23" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="29"/>
-      <c r="E22" s="53" t="s">
+      <c r="D23" s="29"/>
+      <c r="E23" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F23" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="32"/>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="27"/>
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
       <c r="G23" s="31"/>
       <c r="H23" s="31"/>
       <c r="I23" s="31"/>
@@ -1729,8 +1772,8 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
       <c r="D28" s="29"/>
       <c r="E28" s="30"/>
       <c r="F28" s="31"/>
@@ -1765,8 +1808,8 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="27"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="29"/>
       <c r="E31" s="30"/>
       <c r="F31" s="31"/>
@@ -1824,7 +1867,7 @@
       <c r="J35" s="32"/>
     </row>
     <row r="36" spans="1:10">
-      <c r="A36" s="34"/>
+      <c r="A36" s="27"/>
       <c r="B36" s="33"/>
       <c r="C36" s="33"/>
       <c r="D36" s="29"/>
@@ -1848,20 +1891,32 @@
       <c r="J37" s="32"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="40"/>
+      <c r="A38" s="34"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="32"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="35"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:J13"/>
@@ -1875,11 +1930,11 @@
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F54" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F55" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D17 D22:D38" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D17 D23:D39" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Enable output of telegram process list.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7807B6-A886-D847-A6DC-039C191FB71C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669B99E0-6E1D-AB44-AEBD-29608ABA0359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -314,6 +314,69 @@
     </rPh>
     <rPh sb="25" eb="27">
       <t>シテイ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>processlist</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>生成した電文処理のインスタンスを文字列から取得するための配列を生成する場合は、ここにファイル名を指定します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">デンブン </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">ショリ </t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t xml:space="preserve">シュトク </t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t xml:space="preserve">ハイレツ </t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t xml:space="preserve">セイセイ </t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>processlistBase</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>文字列</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>%</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>processList に記述する import 文のbasedirを指定します。</t>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">キジュツ </t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t xml:space="preserve">シテイ </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -847,6 +910,11 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -870,11 +938,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1338,7 +1401,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22:I22"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1383,10 +1446,10 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
@@ -1396,10 +1459,10 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="10" t="s">
         <v>46</v>
       </c>
@@ -1409,10 +1472,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="6" t="s">
         <v>47</v>
       </c>
@@ -1424,10 +1487,10 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
@@ -1461,40 +1524,40 @@
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="62" t="s">
+      <c r="E12" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="F12" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
-      <c r="J12" s="63"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="65"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
-      <c r="H13" s="63"/>
-      <c r="I13" s="63"/>
-      <c r="J13" s="63"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="66"/>
+      <c r="J13" s="66"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="21">
@@ -1608,8 +1671,8 @@
       <c r="I18" s="50"/>
       <c r="J18" s="32"/>
     </row>
-    <row r="19" spans="1:10" s="70" customFormat="1">
-      <c r="A19" s="68">
+    <row r="19" spans="1:10" s="61" customFormat="1">
+      <c r="A19" s="59">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1623,7 +1686,7 @@
       <c r="E19" s="49">
         <v>4</v>
       </c>
-      <c r="F19" s="69" t="s">
+      <c r="F19" s="60" t="s">
         <v>52</v>
       </c>
       <c r="G19" s="50"/>
@@ -1692,12 +1755,12 @@
       <c r="E22" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="59" t="s">
+      <c r="F22" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10">
@@ -1723,24 +1786,42 @@
       <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="27"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
+      <c r="A24" s="27">
+        <v>10</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D24" s="29"/>
       <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
+      <c r="F24" s="31" t="s">
+        <v>54</v>
+      </c>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
       <c r="I24" s="31"/>
       <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="27"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
+      <c r="A25" s="27">
+        <v>11</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>56</v>
+      </c>
       <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
+      <c r="E25" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>58</v>
+      </c>
       <c r="G25" s="31"/>
       <c r="H25" s="31"/>
       <c r="I25" s="31"/>

</xml_diff>

<commit_message>
0.1.11: lineSeparator parameter is implemented to input.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669B99E0-6E1D-AB44-AEBD-29608ABA0359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F59F196-3326-F74D-8788-5623A0988296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -377,6 +377,24 @@
     </rPh>
     <rPh sb="35" eb="37">
       <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>lineSeparator</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>LF</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>行末記号をしていします。LF=0x0a, CR=0x0d, CFLF=0x0d0x0a とします。LFがデフォルトです。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ギョウマツ </t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t xml:space="preserve">キゴウヲ </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -466,7 +484,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -818,11 +836,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="dotted">
+        <color indexed="8"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -937,6 +968,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1329,7 +1369,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1373,7 +1413,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1401,7 +1441,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1828,15 +1868,26 @@
       <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="27"/>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
+      <c r="A26" s="59">
+        <f t="shared" ref="A26" si="1">A25+1</f>
+        <v>12</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="52"/>
+      <c r="E26" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="73"/>
       <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:10">
@@ -1996,7 +2047,8 @@
       <c r="J39" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="F26:I26"/>
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
@@ -2015,7 +2067,7 @@
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D17 D23:D39" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D17 D23:D25 D27:D39" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
0.1.12: searchTmpdir option implemented. Now we can specify object search directory for object searching.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTask.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F59F196-3326-F74D-8788-5623A0988296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DE50C7-B747-2A4A-AA75-3D60C6C65BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -395,6 +395,38 @@
     </rPh>
     <rPh sb="2" eb="4">
       <t xml:space="preserve">キゴウヲ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>searchTmpdir</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>import文作成のために検索するtmpディレクトリをカンマ区切りで指定します。指定ディレクトリ直下のvalueobjectディレクトリの下にxmlを探しにいきます。</t>
+    <rPh sb="6" eb="7">
+      <t xml:space="preserve">ブｎ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">サクセイ </t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t xml:space="preserve">ケンサク </t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t xml:space="preserve">チョッカ </t>
+    </rPh>
+    <rPh sb="69" eb="70">
+      <t xml:space="preserve">シタニ </t>
+    </rPh>
+    <rPh sb="75" eb="76">
+      <t xml:space="preserve">サガシニ </t>
     </rPh>
     <phoneticPr fontId="5"/>
   </si>
@@ -946,6 +978,25 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -958,25 +1009,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1438,10 +1470,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1486,10 +1518,10 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="67"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
@@ -1499,10 +1531,10 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="67"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="10" t="s">
         <v>46</v>
       </c>
@@ -1512,10 +1544,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="67"/>
+      <c r="B8" s="64"/>
       <c r="C8" s="6" t="s">
         <v>47</v>
       </c>
@@ -1527,10 +1559,10 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="67"/>
+      <c r="B9" s="64"/>
       <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
@@ -1564,40 +1596,40 @@
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="69" t="s">
+      <c r="C12" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="64" t="s">
+      <c r="D12" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="65" t="s">
+      <c r="E12" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="66" t="s">
+      <c r="F12" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="66"/>
-      <c r="J12" s="66"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="68"/>
-      <c r="B13" s="68"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="66"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="21">
@@ -1795,12 +1827,12 @@
       <c r="E22" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="62" t="s">
+      <c r="F22" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
-      <c r="I22" s="63"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10">
@@ -1869,7 +1901,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="59">
-        <f t="shared" ref="A26" si="1">A25+1</f>
+        <f t="shared" ref="A26:A27" si="1">A25+1</f>
         <v>12</v>
       </c>
       <c r="B26" s="51" t="s">
@@ -1882,21 +1914,30 @@
       <c r="E26" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="71" t="s">
+      <c r="F26" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="73"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="68"/>
       <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="27"/>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
+      <c r="A27" s="27">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D27" s="29"/>
       <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
+      <c r="F27" s="31" t="s">
+        <v>63</v>
+      </c>
       <c r="G27" s="31"/>
       <c r="H27" s="31"/>
       <c r="I27" s="31"/>
@@ -1916,8 +1957,8 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
       <c r="D29" s="29"/>
       <c r="E29" s="30"/>
       <c r="F29" s="31"/>
@@ -1952,8 +1993,8 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="27"/>
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="29"/>
       <c r="E32" s="30"/>
       <c r="F32" s="31"/>
@@ -2011,7 +2052,7 @@
       <c r="J36" s="32"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="34"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="33"/>
       <c r="C37" s="33"/>
       <c r="D37" s="29"/>
@@ -2035,16 +2076,28 @@
       <c r="J38" s="32"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="35"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="39"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="40"/>
+      <c r="A39" s="34"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="31"/>
+      <c r="J39" s="32"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="35"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="37"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2053,21 +2106,21 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:J13"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F55" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F56" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D17 D23:D25 D27:D39" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D17 D23:D25 D27:D40" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
0.1.15: Generate toJSON method on telegram classes.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTask.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DE50C7-B747-2A4A-AA75-3D60C6C65BA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B3A1313-288F-704F-AD64-A2C78FE8F59B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7720" yWindow="760" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14240" yWindow="2420" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anttask" sheetId="1" r:id="rId1"/>
     <sheet name="config" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="Submit有無">#REF!</definedName>
     <definedName name="Validate実装パターン">#REF!</definedName>
@@ -23,6 +26,7 @@
     <definedName name="デリミタ">#REF!</definedName>
     <definedName name="デリミタ選択肢">#REF!</definedName>
     <definedName name="型">#REF!</definedName>
+    <definedName name="型リスト">[1]config!$A$5:$A$12</definedName>
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">config!$C$5:$C$6</definedName>
   </definedNames>
@@ -41,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -428,6 +432,14 @@
     <rPh sb="75" eb="76">
       <t xml:space="preserve">サガシニ </t>
     </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>generateToJson</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>toJSONメソッドを生成します</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -978,16 +990,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1008,6 +1010,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1093,6 +1105,47 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="anttask"/>
+      <sheetName val="config"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>文字列</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>整数(int)</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>整数(long)</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>数値(decimal)</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>真偽</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1401,7 +1454,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1445,7 +1498,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1473,7 +1526,7 @@
   <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1518,10 +1571,10 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="64"/>
+      <c r="B6" s="72"/>
       <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
@@ -1531,10 +1584,10 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="72"/>
       <c r="C7" s="10" t="s">
         <v>46</v>
       </c>
@@ -1544,10 +1597,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="72"/>
       <c r="C8" s="6" t="s">
         <v>47</v>
       </c>
@@ -1559,10 +1612,10 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="64"/>
+      <c r="B9" s="72"/>
       <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
@@ -1596,40 +1649,40 @@
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="72" t="s">
+      <c r="E12" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="73" t="s">
+      <c r="F12" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="73"/>
-      <c r="J12" s="73"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="65"/>
-      <c r="B13" s="65"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="73"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="73"/>
-      <c r="J13" s="73"/>
+      <c r="A13" s="73"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="21">
@@ -1827,12 +1880,12 @@
       <c r="E22" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="69" t="s">
+      <c r="F22" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="70"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10">
@@ -1901,7 +1954,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="59">
-        <f t="shared" ref="A26:A27" si="1">A25+1</f>
+        <f t="shared" ref="A26:A28" si="1">A25+1</f>
         <v>12</v>
       </c>
       <c r="B26" s="51" t="s">
@@ -1914,12 +1967,12 @@
       <c r="E26" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="66" t="s">
+      <c r="F26" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="68"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="64"/>
       <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:10">
@@ -1944,12 +1997,23 @@
       <c r="J27" s="32"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="27"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
+      <c r="A28" s="27">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
+      <c r="E28" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>65</v>
+      </c>
       <c r="G28" s="31"/>
       <c r="H28" s="31"/>
       <c r="I28" s="31"/>
@@ -2101,11 +2165,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:J13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
@@ -2113,6 +2172,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:J13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
0.2.7: Enable to specify ApiTelegrams package (setting dir) as ant task parameter.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A454FA-7892-0644-B53E-2950D3745556}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D98983A-FF95-684B-AF5E-1792D0341F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14240" yWindow="2420" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -440,6 +440,52 @@
   </si>
   <si>
     <t>toJSONメソッドを生成します</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>電文の親クラスの配置場所を、Javaのパッケージ形式で指定します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">オヤクラス </t>
+    </rPh>
+    <rPh sb="8" eb="12">
+      <t xml:space="preserve">ハイチバショヲ </t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t xml:space="preserve">ケイシキ </t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>apiTelegramPackage</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>apiTelegramBase</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>電文の親クラスの配置場所のaliasを指定します。通常は % です。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">デンブｎ </t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ノ</t>
+    </rPh>
+    <rPh sb="3" eb="7">
+      <t>オヤｋ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t xml:space="preserve">ツウジョウハ </t>
+    </rPh>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1525,8 +1571,8 @@
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1731,7 +1777,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="27">
-        <f t="shared" ref="A16:A28" si="0">A15+1</f>
+        <f t="shared" ref="A16:A30" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="28" t="s">
@@ -2023,24 +2069,44 @@
       <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="27"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
+      <c r="A29" s="59">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D29" s="29"/>
       <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
+      <c r="F29" s="31" t="s">
+        <v>66</v>
+      </c>
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
       <c r="I29" s="31"/>
       <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="59">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="45" t="s">
+        <v>33</v>
+      </c>
       <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
+      <c r="E30" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F30" s="31" t="s">
+        <v>69</v>
+      </c>
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
       <c r="I30" s="31"/>

</xml_diff>

<commit_message>
3.1.9: Implement stringifyObjectQuery and stringifyArrayQuery options.
on true stringifyObjectQuery, object and array of object query parameters are JSON stringified.
on addition, true stringifyArrayQuery, primitive array also JSON stringified.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoRestGeneratorTsTask.xlsx
+++ b/meta/program/BlancoRestGeneratorTsTask.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoRestGeneratorTs/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE4458D-E9C5-3D4F-A5A0-2E9D6E42235D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA83602A-4C63-2D4C-8BB6-938138488342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14240" yWindow="2420" windowWidth="21080" windowHeight="17240" tabRatio="860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t>AntTask定義書</t>
   </si>
@@ -516,6 +516,85 @@
     <rPh sb="34" eb="36">
       <t xml:space="preserve">ウワガキ </t>
     </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>クエリ文字列にObjectが指定された場合はJSON文字列化して渡す。配列の要素がprimitiveでない場合は配列全体をJSON化する。</t>
+    <rPh sb="3" eb="6">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="26" eb="29">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t xml:space="preserve">カ </t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t xml:space="preserve">ワタス </t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t xml:space="preserve">ハイレツ </t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t xml:space="preserve">ヨウソガ </t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t xml:space="preserve">バアイ </t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t xml:space="preserve">ハイレツ </t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t xml:space="preserve">ゼンタイ </t>
+    </rPh>
+    <rPh sb="65" eb="66">
+      <t xml:space="preserve">カ </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>クエリ文字列に配列が指定された場合は配列全体をJSON文字列化して渡す</t>
+    <rPh sb="0" eb="3">
+      <t>クエリム</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t xml:space="preserve">ハイレツガ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t xml:space="preserve">バアイハ </t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t xml:space="preserve">ハイレツ </t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t xml:space="preserve">ゼンタイヲ </t>
+    </rPh>
+    <rPh sb="27" eb="31">
+      <t xml:space="preserve">モジレツカ </t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t xml:space="preserve">ワタス </t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>stringifyObjectQuery</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>stringifyArrayQuery</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -1063,16 +1142,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1093,6 +1162,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1527,7 +1606,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1571,7 +1650,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -1596,10 +1675,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1644,10 +1723,10 @@
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="59"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
@@ -1657,10 +1736,10 @@
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="59"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="10" t="s">
         <v>46</v>
       </c>
@@ -1670,10 +1749,10 @@
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="6" t="s">
         <v>47</v>
       </c>
@@ -1685,10 +1764,10 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="59"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="13" t="s">
         <v>9</v>
       </c>
@@ -1722,40 +1801,40 @@
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="13.5" customHeight="1">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="68" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="67" t="s">
+      <c r="E12" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="68" t="s">
+      <c r="F12" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="16">
@@ -1804,7 +1883,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="22">
-        <f t="shared" ref="A16:A32" si="0">A15+1</f>
+        <f t="shared" ref="A16:A34" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -1953,12 +2032,12 @@
       <c r="E22" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="64" t="s">
+      <c r="F22" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
       <c r="J22" s="27"/>
     </row>
     <row r="23" spans="1:10">
@@ -2043,12 +2122,12 @@
       <c r="E26" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="F26" s="61" t="s">
+      <c r="F26" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="63"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
       <c r="J26" s="27"/>
     </row>
     <row r="27" spans="1:10">
@@ -2186,24 +2265,46 @@
       <c r="J32" s="27"/>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="22"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
+      <c r="A33" s="53">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>34</v>
+      </c>
       <c r="D33" s="24"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="26"/>
+      <c r="E33" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>74</v>
+      </c>
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
       <c r="J33" s="27"/>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="22"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="53">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>34</v>
+      </c>
       <c r="D34" s="24"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="26"/>
+      <c r="E34" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>75</v>
+      </c>
       <c r="G34" s="26"/>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -2258,7 +2359,7 @@
       <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10">
-      <c r="A39" s="29"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
       <c r="D39" s="24"/>
@@ -2282,24 +2383,31 @@
       <c r="J40" s="27"/>
     </row>
     <row r="41" spans="1:10">
-      <c r="A41" s="30"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
-      <c r="J41" s="35"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="27"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="30"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:J13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
@@ -2307,14 +2415,19 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:J13"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F57" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F58" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D17 D23:D25 D27:D41" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" operator="equal" allowBlank="1" sqref="D14:D17 D23:D25 D27:D42" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>必須</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>